<commit_message>
Bakery and Manor House 1 configured
</commit_message>
<xml_diff>
--- a/Assets/Spritesheets/Configuration Status.xlsx
+++ b/Assets/Spritesheets/Configuration Status.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuwij/UnityProjects/Macabre/Assets/Spritesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64749938-E84E-AF48-B6D5-3035DA509BD9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E20758E-4C51-7C4F-A608-7B9B37730443}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{A46E6C7B-4771-4E49-B2E1-919B5DFBBBA0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rooms" sheetId="1" r:id="rId1"/>
+    <sheet name="Characters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="53">
   <si>
     <t>Room</t>
   </si>
@@ -169,6 +170,21 @@
   </si>
   <si>
     <t>ManorHouse 3 Floor 2 Room 1</t>
+  </si>
+  <si>
+    <t>Ladder needs footprint</t>
+  </si>
+  <si>
+    <t>Door needs footprint, split up boxes or make one collier for all</t>
+  </si>
+  <si>
+    <t>Ladder missing rightmost pixel</t>
+  </si>
+  <si>
+    <t>Seat missing rightmost pixel, Chest missing rightmost pixel</t>
+  </si>
+  <si>
+    <t>Missing rightmost pixel for most objects</t>
   </si>
 </sst>
 </file>
@@ -233,27 +249,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -275,6 +271,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>172138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C013239-B8A6-8A46-98A4-382208B95467}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14643100" y="1772338"/>
+          <a:ext cx="2794000" cy="2037662"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>467745</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FDCE4ED-4581-E44B-8423-6AD99E149C51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17602200" y="1828800"/>
+          <a:ext cx="2880745" cy="2019300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>718868</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>368299</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8ED6FE1-D0B0-114A-A422-0A9C93E6F8BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14955568" y="4127500"/>
+          <a:ext cx="4602431" cy="2057400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,7 +710,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,15 +1011,24 @@
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
+      <c r="K11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -898,15 +1040,24 @@
       <c r="C12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
+      <c r="K12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -918,15 +1069,24 @@
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
+      <c r="K13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -938,12 +1098,18 @@
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -962,11 +1128,18 @@
       <c r="E15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
+      <c r="K15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -982,11 +1155,16 @@
       <c r="E16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1347,11 +1525,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:J262">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC42614-0061-DB41-9C39-713DF8CC7295}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all characters, exept animations
</commit_message>
<xml_diff>
--- a/Assets/Spritesheets/Configuration Status.xlsx
+++ b/Assets/Spritesheets/Configuration Status.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuwij/UnityProjects/Macabre/Assets/Spritesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6322DBAB-E4C1-F241-8525-92483B16F11C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFA0A93-C6E4-E84D-A47A-1BE266B80BD6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{A46E6C7B-4771-4E49-B2E1-919B5DFBBBA0}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="Room Design" sheetId="1" r:id="rId1"/>
     <sheet name="Character Design" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,8 +25,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jiashen Wang</author>
+  </authors>
+  <commentList>
+    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{8FC87234-34B6-A54E-9F68-15FC23FB8958}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jiashen Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rohez Spirtehseet not the same as others</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="107">
   <si>
     <t>Room</t>
   </si>
@@ -248,9 +280,6 @@
     <t>JohanTheLibrarian</t>
   </si>
   <si>
-    <t>JohnTheSon</t>
-  </si>
-  <si>
     <t>MackenzieThePriest</t>
   </si>
   <si>
@@ -330,13 +359,34 @@
   </si>
   <si>
     <t>Ground Pickup</t>
+  </si>
+  <si>
+    <t>Cloakguy 1</t>
+  </si>
+  <si>
+    <t>Cloakguy 2</t>
+  </si>
+  <si>
+    <t>Cloakguy 3</t>
+  </si>
+  <si>
+    <t>Cloakguy 4</t>
+  </si>
+  <si>
+    <t>Cloakguy 5</t>
+  </si>
+  <si>
+    <t>Uploaded</t>
+  </si>
+  <si>
+    <t>JohnTheCoward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +408,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -483,11 +546,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="8" tint="-0.24994659260841701"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -538,6 +606,86 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1236,6 +1384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB317F25-C013-CC4F-9B42-9988FD75637D}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1277,7 +1426,7 @@
         <v>33</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>34</v>
@@ -1532,16 +1681,16 @@
         <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2046,7 +2195,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>32</v>
@@ -2271,12 +2420,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K26 B28:K263 J27:K27">
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:I27">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2287,11 +2436,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D6B528-233C-A94C-BFE0-99E0B5C73C5B}">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D6B528-233C-A94C-BFE0-99E0B5C73C5B}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2317,22 +2467,22 @@
         <v>59</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2340,13 +2490,13 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2359,110 +2509,116 @@
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>
@@ -2476,26 +2632,32 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>95</v>
@@ -2503,226 +2665,297 @@
       <c r="C16" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>95</v>
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>105</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" t="s">
-        <v>96</v>
+        <v>76</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>95</v>
+        <v>77</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H32" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" t="s">
+        <v>94</v>
+      </c>
+      <c r="J32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H27" t="s">
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="14"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" t="s">
         <v>95</v>
       </c>
-      <c r="I27" t="s">
-        <v>95</v>
-      </c>
-      <c r="J27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+      <c r="H36" t="s">
         <v>91</v>
       </c>
-      <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G31" t="s">
-        <v>92</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A28">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Complete">
+  <conditionalFormatting sqref="A3:A34">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD18 A19:A20 E19:XFD20 A21:XFD1048576">
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Lined">
+  <conditionalFormatting sqref="A24:A25 E24:XFD25 A26:XFD1048576 A1:XFD23">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Designed">
+      <formula>NOT(ISERROR(SEARCH("Designed",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Tested">
+      <formula>NOT(ISERROR(SEARCH("Tested",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Animated">
+      <formula>NOT(ISERROR(SEARCH("Animated",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Shaded">
+      <formula>NOT(ISERROR(SEARCH("Shaded",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Colored">
+      <formula>NOT(ISERROR(SEARCH("Colored",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Lined">
       <formula>NOT(ISERROR(SEARCH("Lined",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Colored">
-      <formula>NOT(ISERROR(SEARCH("Colored",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Shaded">
-      <formula>NOT(ISERROR(SEARCH("Shaded",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Animated">
-      <formula>NOT(ISERROR(SEARCH("Animated",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Tested">
-      <formula>NOT(ISERROR(SEARCH("Tested",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Designed">
-      <formula>NOT(ISERROR(SEARCH("Designed",A1)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Uploaded">
+      <formula>NOT(ISERROR(SEARCH("Uploaded",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Multibody pixel collider
</commit_message>
<xml_diff>
--- a/Assets/Spritesheets/Configuration Status.xlsx
+++ b/Assets/Spritesheets/Configuration Status.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuwij/UnityProjects/Macabre/Assets/Spritesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F6A3B6-25EF-F644-891A-95D57CC08CD1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BB614-8CBB-F64F-9F16-0A54D46EF740}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{A46E6C7B-4771-4E49-B2E1-919B5DFBBBA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Room Design" sheetId="1" r:id="rId1"/>
-    <sheet name="Character Design" sheetId="3" r:id="rId2"/>
+    <sheet name="Overworld Objects" sheetId="4" r:id="rId2"/>
+    <sheet name="Character Design" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="125">
   <si>
     <t>Room</t>
   </si>
@@ -383,6 +384,57 @@
   </si>
   <si>
     <t>Guard</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Objects</t>
+  </si>
+  <si>
+    <t>Docks</t>
+  </si>
+  <si>
+    <t>Bakery Exterior</t>
+  </si>
+  <si>
+    <t>Shack Exterior</t>
+  </si>
+  <si>
+    <t>Vineyard Exterior</t>
+  </si>
+  <si>
+    <t>Guardhouse Exterior</t>
+  </si>
+  <si>
+    <t>Inn Exterior</t>
+  </si>
+  <si>
+    <t>Church Exterior</t>
+  </si>
+  <si>
+    <t>Blacksmith Exterior</t>
+  </si>
+  <si>
+    <t>ManorHouse 1 Exterior</t>
+  </si>
+  <si>
+    <t>ManorHouse 2 Exterior</t>
+  </si>
+  <si>
+    <t>ManorHouse 3 Exterior</t>
+  </si>
+  <si>
+    <t>Customs House Exterior</t>
+  </si>
+  <si>
+    <t>Collision Body Created</t>
+  </si>
+  <si>
+    <t>Doors Created</t>
+  </si>
+  <si>
+    <t>Sprites Created</t>
   </si>
 </sst>
 </file>
@@ -549,7 +601,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -612,6 +674,46 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2348,12 +2450,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K26 B28:K263 J27:K27">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:I27">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2364,12 +2466,160 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD6C431-A7BC-9C40-9053-84CF2EB47EBA}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="17" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="5" customWidth="1"/>
+    <col min="5" max="15" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:S40">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D6B528-233C-A94C-BFE0-99E0B5C73C5B}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2866,34 +3116,42 @@
       <c r="H37" t="s">
         <v>91</v>
       </c>
+      <c r="J37" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A35">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A25 E24:XFD25 A1:XFD23 A26:XFD31 A32:G33 K32:XFD33 A34:XFD1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Uploaded">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Uploaded">
       <formula>NOT(ISERROR(SEARCH("Uploaded",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Designed">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Designed">
       <formula>NOT(ISERROR(SEARCH("Designed",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Tested">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Tested">
       <formula>NOT(ISERROR(SEARCH("Tested",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Animated">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Animated">
       <formula>NOT(ISERROR(SEARCH("Animated",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Shaded">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Shaded">
       <formula>NOT(ISERROR(SEARCH("Shaded",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Colored">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Colored">
       <formula>NOT(ISERROR(SEARCH("Colored",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Lined">
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="Lined">
       <formula>NOT(ISERROR(SEARCH("Lined",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:XFD183">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Bug">
+      <formula>NOT(ISERROR(SEARCH("Bug",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Multiobject sorting with shadows and transparency
</commit_message>
<xml_diff>
--- a/Assets/Spritesheets/Configuration Status.xlsx
+++ b/Assets/Spritesheets/Configuration Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuwij/UnityProjects/Macabre/Assets/Spritesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BB614-8CBB-F64F-9F16-0A54D46EF740}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A7EF7-AFE7-284E-B1F0-26F5614A7F32}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{A46E6C7B-4771-4E49-B2E1-919B5DFBBBA0}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="125">
   <si>
     <t>Room</t>
   </si>
@@ -601,7 +601,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -674,36 +674,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2470,7 +2440,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2522,6 +2492,9 @@
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2530,6 +2503,9 @@
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2538,6 +2514,9 @@
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2546,6 +2525,9 @@
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -2554,6 +2536,9 @@
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2562,6 +2547,9 @@
       <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2570,6 +2558,9 @@
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2578,6 +2569,9 @@
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2586,6 +2580,9 @@
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2594,12 +2591,18 @@
       <c r="B13" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Door to bakery done:
</commit_message>
<xml_diff>
--- a/Assets/Spritesheets/Configuration Status.xlsx
+++ b/Assets/Spritesheets/Configuration Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuwij/UnityProjects/Macabre/Assets/Spritesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A7EF7-AFE7-284E-B1F0-26F5614A7F32}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE6D5BF3-B647-E249-B7A5-B4F022FD1BA5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{A46E6C7B-4771-4E49-B2E1-919B5DFBBBA0}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Character Design" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="132">
   <si>
     <t>Room</t>
   </si>
@@ -435,6 +436,27 @@
   </si>
   <si>
     <t>Sprites Created</t>
+  </si>
+  <si>
+    <t>Shadow Added</t>
+  </si>
+  <si>
+    <t>Exterior Objects Created</t>
+  </si>
+  <si>
+    <t>Missing Frontal Sprite</t>
+  </si>
+  <si>
+    <t>Needs sprite covering floor</t>
+  </si>
+  <si>
+    <t>Test Sorting</t>
+  </si>
+  <si>
+    <t>Shadow needs to include back portion</t>
+  </si>
+  <si>
+    <t>Think backside part of shadow is incorrect (Fig 1)</t>
   </si>
 </sst>
 </file>
@@ -1087,6 +1109,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5B4BF66-9ACC-0246-9281-0D55178F7335}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12992100" y="1816100"/>
+          <a:ext cx="7442200" cy="4635500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2437,22 +2508,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD6C431-A7BC-9C40-9053-84CF2EB47EBA}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="17" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="5" customWidth="1"/>
-    <col min="5" max="15" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="42.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="5" customWidth="1"/>
+    <col min="7" max="16" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>109</v>
       </c>
@@ -2460,13 +2533,19 @@
         <v>124</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -2476,16 +2555,25 @@
       <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -2495,8 +2583,11 @@
       <c r="C4" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -2506,8 +2597,11 @@
       <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -2515,10 +2609,13 @@
         <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -2528,8 +2625,11 @@
       <c r="C7" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -2537,10 +2637,13 @@
         <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2550,8 +2653,11 @@
       <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -2561,8 +2667,14 @@
       <c r="C10" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -2572,8 +2684,11 @@
       <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -2581,10 +2696,13 @@
         <v>32</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2592,10 +2710,13 @@
         <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -2605,14 +2726,18 @@
       <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:S40">
+  <conditionalFormatting sqref="B2:T40">
     <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed a few things
</commit_message>
<xml_diff>
--- a/Assets/Spritesheets/Configuration Status.xlsx
+++ b/Assets/Spritesheets/Configuration Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Pictures\Working Files\Macabre\Macabre\Assets\Spritesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0288E847-863E-4654-92CF-E0B42523EFAB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F516DD15-BCAC-4629-B05F-848D70A11FB9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="2" xr2:uid="{A46E6C7B-4771-4E49-B2E1-919B5DFBBBA0}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="132">
   <si>
     <t>Room</t>
   </si>
@@ -462,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -474,13 +474,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF305496"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,18 +492,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -591,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,7 +599,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -622,7 +608,137 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2490,12 +2606,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K26 B28:K263 J27:K27">
-    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:I27">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2731,7 +2847,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:T40">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2745,21 +2861,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="25.5" style="14" customWidth="1"/>
     <col min="2" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
+      <c r="A1" s="10"/>
     </row>
     <row r="2" spans="1:10" s="7" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2791,7 +2907,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B3" t="s">
@@ -2805,7 +2921,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B4" t="s">
@@ -2819,21 +2935,21 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>100</v>
       </c>
       <c r="B6" t="s">
@@ -2847,7 +2963,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B7" t="s">
@@ -2861,7 +2977,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>102</v>
       </c>
       <c r="B8" t="s">
@@ -2875,7 +2991,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="B9" t="s">
@@ -2889,7 +3005,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>104</v>
       </c>
       <c r="B10" t="s">
@@ -2903,21 +3019,21 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B12" t="s">
@@ -2931,7 +3047,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B13" t="s">
@@ -2945,32 +3061,32 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B16" t="s">
@@ -2984,18 +3100,18 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B18" t="s">
@@ -3009,21 +3125,21 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B20" t="s">
@@ -3037,7 +3153,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>106</v>
       </c>
       <c r="B21" t="s">
@@ -3052,21 +3168,21 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>94</v>
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>74</v>
       </c>
       <c r="B23" t="s">
@@ -3078,51 +3194,54 @@
       <c r="D23" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>94</v>
+      <c r="F23" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>94</v>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>94</v>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B27" t="s">
@@ -3136,21 +3255,21 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B29" t="s">
@@ -3164,7 +3283,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>82</v>
       </c>
       <c r="B30" t="s">
@@ -3178,52 +3297,52 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>94</v>
+        <v>105</v>
+      </c>
+      <c r="G31" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>85</v>
       </c>
       <c r="B34" t="s">
@@ -3246,7 +3365,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="13"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -3276,36 +3395,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A35">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A25 E24:XFD25 A26:XFD31 K32:XFD33 A34:XFD1048576 A1:XFD23 A32:G33">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Uploaded">
+  <conditionalFormatting sqref="A24:A25 E24:XFD25 K32:XFD33 A34:XFD1048576 A32:G33 A1:XFD23 A26:XFD31">
+    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Uploaded">
       <formula>NOT(ISERROR(SEARCH("Uploaded",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Designed">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="Designed">
       <formula>NOT(ISERROR(SEARCH("Designed",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Tested">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Tested">
       <formula>NOT(ISERROR(SEARCH("Tested",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Animated">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Animated">
       <formula>NOT(ISERROR(SEARCH("Animated",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Shaded">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Shaded">
       <formula>NOT(ISERROR(SEARCH("Shaded",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Colored">
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="Colored">
       <formula>NOT(ISERROR(SEARCH("Colored",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="Lined">
+    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="Lined">
       <formula>NOT(ISERROR(SEARCH("Lined",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD183">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Bug">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Bug">
       <formula>NOT(ISERROR(SEARCH("Bug",A3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:D25">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Uploaded">
+      <formula>NOT(ISERROR(SEARCH("Uploaded",B25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Designed">
+      <formula>NOT(ISERROR(SEARCH("Designed",B25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Tested">
+      <formula>NOT(ISERROR(SEARCH("Tested",B25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Animated">
+      <formula>NOT(ISERROR(SEARCH("Animated",B25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Shaded">
+      <formula>NOT(ISERROR(SEARCH("Shaded",B25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="Colored">
+      <formula>NOT(ISERROR(SEARCH("Colored",B25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="Lined">
+      <formula>NOT(ISERROR(SEARCH("Lined",B25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:D24">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Uploaded">
+      <formula>NOT(ISERROR(SEARCH("Uploaded",B24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Designed">
+      <formula>NOT(ISERROR(SEARCH("Designed",B24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Tested">
+      <formula>NOT(ISERROR(SEARCH("Tested",B24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Animated">
+      <formula>NOT(ISERROR(SEARCH("Animated",B24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Shaded">
+      <formula>NOT(ISERROR(SEARCH("Shaded",B24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Colored">
+      <formula>NOT(ISERROR(SEARCH("Colored",B24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Lined">
+      <formula>NOT(ISERROR(SEARCH("Lined",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>